<commit_message>
final merge with develoopment-Sagar
</commit_message>
<xml_diff>
--- a/Gantt Chart.xlsx
+++ b/Gantt Chart.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimishathakkar/Downloads/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B379109C-026D-EF43-B796-BF02C997854D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="24240" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="Progress as on date" sheetId="1" r:id="rId1"/>
@@ -18,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Progress as on date'!$A$1:$J$28</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>Description</t>
   </si>
@@ -126,9 +120,6 @@
     <t>Updated the sensor shape</t>
   </si>
   <si>
-    <t>UNIT TESTING</t>
-  </si>
-  <si>
     <t>Coding</t>
   </si>
   <si>
@@ -138,19 +129,40 @@
     <t>Added some changes to the previous file to improve the functionality</t>
   </si>
   <si>
-    <t>Tested the car model by integrating the kivy file with the python file and made changes in the code accordingly</t>
+    <t>Sr. No.</t>
   </si>
   <si>
-    <t>Learning the algorithms of deep learning and started working on "ai.py" file</t>
+    <t>W-9</t>
   </si>
   <si>
-    <t>Sr. No.</t>
+    <t>W-10</t>
+  </si>
+  <si>
+    <t>W-11</t>
+  </si>
+  <si>
+    <t>W-12</t>
+  </si>
+  <si>
+    <t>Implemented Deep learning architecture and Q-learning functions for the brain of self driving car</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TESTING</t>
+  </si>
+  <si>
+    <t>Performed Unit testing for base layer and q-learning modules</t>
+  </si>
+  <si>
+    <t>Integrated graphics with the brain of AI and performed integration testing</t>
+  </si>
+  <si>
+    <t>Merged  all modules and performed system testing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -260,7 +272,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -542,21 +554,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -619,17 +616,173 @@
       <right style="thin">
         <color indexed="8"/>
       </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
       <top style="thin">
         <color indexed="8"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
+      <bottom style="thin">
+        <color indexed="8"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color indexed="8"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="8"/>
@@ -637,81 +790,25 @@
       <top style="thin">
         <color indexed="8"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color indexed="8"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="8"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -729,7 +826,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -761,47 +857,33 @@
     <xf numFmtId="16" fontId="4" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="4" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="5" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -839,12 +921,66 @@
     <xf numFmtId="10" fontId="7" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="4" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2034,158 +2170,190 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:IZ28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IX31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A25" sqref="A25"/>
+      <selection pane="bottomRight" activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="59" style="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.1640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5" style="1" customWidth="1"/>
-    <col min="11" max="27" width="9.1640625" style="12" customWidth="1"/>
-    <col min="28" max="260" width="9.1640625" style="13"/>
+    <col min="4" max="4" width="9.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" style="1" customWidth="1"/>
+    <col min="11" max="17" width="9.140625" style="12" customWidth="1"/>
+    <col min="18" max="250" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:260" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:258" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="55" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="53" t="s">
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="20"/>
-      <c r="J1" s="21" t="s">
+      <c r="I1" s="19"/>
+      <c r="J1" s="20" t="s">
         <v>15</v>
       </c>
+      <c r="K1" s="57"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="59"/>
     </row>
-    <row r="2" spans="1:260" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="51"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="21" t="s">
+    <row r="2" spans="1:258" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="42"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="20" t="s">
         <v>17</v>
       </c>
+      <c r="K2" s="60"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+      <c r="N2" s="62"/>
     </row>
-    <row r="3" spans="1:260" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="51"/>
-      <c r="B3" s="52"/>
-      <c r="C3" s="23" t="s">
+    <row r="3" spans="1:258" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="42"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="25" t="s">
+      <c r="I3" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="24" t="s">
+      <c r="J3" s="23" t="s">
         <v>13</v>
       </c>
+      <c r="K3" s="56" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="56" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" s="56" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="4" spans="1:260" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="27" t="s">
+    <row r="4" spans="1:258" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="28">
+      <c r="C4" s="27">
         <v>43845</v>
       </c>
-      <c r="D4" s="28">
+      <c r="D4" s="27">
         <v>43852</v>
       </c>
-      <c r="E4" s="28">
+      <c r="E4" s="27">
         <v>43859</v>
       </c>
-      <c r="F4" s="28">
+      <c r="F4" s="27">
         <v>43866</v>
       </c>
-      <c r="G4" s="28">
+      <c r="G4" s="27">
         <v>43873</v>
       </c>
-      <c r="H4" s="28">
+      <c r="H4" s="27">
         <v>43880</v>
       </c>
-      <c r="I4" s="28">
+      <c r="I4" s="27">
         <v>43887</v>
       </c>
-      <c r="J4" s="29">
+      <c r="J4" s="27">
         <v>43894</v>
       </c>
+      <c r="K4" s="55">
+        <v>43901</v>
+      </c>
+      <c r="L4" s="55">
+        <v>43908</v>
+      </c>
+      <c r="M4" s="55">
+        <v>43915</v>
+      </c>
+      <c r="N4" s="55">
+        <v>43922</v>
+      </c>
     </row>
-    <row r="5" spans="1:260" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="62" t="s">
+    <row r="5" spans="1:258" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="52"/>
+      <c r="L5" s="53"/>
+      <c r="M5" s="53"/>
+      <c r="N5" s="53"/>
       <c r="O5" s="12"/>
       <c r="P5" s="12"/>
       <c r="Q5" s="12"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="12"/>
-      <c r="T5" s="12"/>
-      <c r="U5" s="12"/>
-      <c r="V5" s="12"/>
-      <c r="W5" s="12"/>
-      <c r="X5" s="12"/>
-      <c r="Y5" s="12"/>
-      <c r="Z5" s="12"/>
-      <c r="AA5" s="12"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="13"/>
+      <c r="U5" s="13"/>
+      <c r="V5" s="13"/>
+      <c r="W5" s="13"/>
+      <c r="X5" s="13"/>
+      <c r="Y5" s="13"/>
+      <c r="Z5" s="13"/>
+      <c r="AA5" s="13"/>
       <c r="AB5" s="13"/>
       <c r="AC5" s="13"/>
       <c r="AD5" s="13"/>
@@ -2409,20 +2577,10 @@
       <c r="IN5" s="13"/>
       <c r="IO5" s="13"/>
       <c r="IP5" s="13"/>
-      <c r="IQ5" s="13"/>
-      <c r="IR5" s="13"/>
-      <c r="IS5" s="13"/>
-      <c r="IT5" s="13"/>
-      <c r="IU5" s="13"/>
-      <c r="IV5" s="13"/>
-      <c r="IW5" s="13"/>
-      <c r="IX5" s="13"/>
-      <c r="IY5" s="13"/>
-      <c r="IZ5" s="13"/>
     </row>
-    <row r="6" spans="1:260" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="44"/>
-      <c r="B6" s="45"/>
+    <row r="6" spans="1:258" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="36"/>
+      <c r="B6" s="37"/>
       <c r="C6" s="8"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -2430,13 +2588,17 @@
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="31"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
     </row>
-    <row r="7" spans="1:260" ht="46" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="32">
+    <row r="7" spans="1:258" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="30">
         <v>1</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="9"/>
@@ -2446,40 +2608,44 @@
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
-      <c r="J7" s="33"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
     </row>
-    <row r="8" spans="1:260" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="62" t="s">
+    <row r="8" spans="1:258" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="61" t="s">
+      <c r="B8" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="52"/>
+      <c r="L8" s="53"/>
+      <c r="M8" s="53"/>
+      <c r="N8" s="53"/>
       <c r="O8" s="12"/>
       <c r="P8" s="12"/>
       <c r="Q8" s="12"/>
-      <c r="R8" s="12"/>
-      <c r="S8" s="12"/>
-      <c r="T8" s="12"/>
-      <c r="U8" s="12"/>
-      <c r="V8" s="12"/>
-      <c r="W8" s="12"/>
-      <c r="X8" s="12"/>
-      <c r="Y8" s="12"/>
-      <c r="Z8" s="12"/>
-      <c r="AA8" s="12"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="13"/>
+      <c r="W8" s="13"/>
+      <c r="X8" s="13"/>
+      <c r="Y8" s="13"/>
+      <c r="Z8" s="13"/>
+      <c r="AA8" s="13"/>
       <c r="AB8" s="13"/>
       <c r="AC8" s="13"/>
       <c r="AD8" s="13"/>
@@ -2703,19 +2869,9 @@
       <c r="IN8" s="13"/>
       <c r="IO8" s="13"/>
       <c r="IP8" s="13"/>
-      <c r="IQ8" s="13"/>
-      <c r="IR8" s="13"/>
-      <c r="IS8" s="13"/>
-      <c r="IT8" s="13"/>
-      <c r="IU8" s="13"/>
-      <c r="IV8" s="13"/>
-      <c r="IW8" s="13"/>
-      <c r="IX8" s="13"/>
-      <c r="IY8" s="13"/>
-      <c r="IZ8" s="13"/>
     </row>
-    <row r="9" spans="1:260" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="30"/>
+    <row r="9" spans="1:258" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="28"/>
       <c r="B9" s="3"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -2724,13 +2880,17 @@
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
-      <c r="J9" s="31"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="66"/>
+      <c r="L9" s="66"/>
+      <c r="M9" s="66"/>
+      <c r="N9" s="66"/>
     </row>
-    <row r="10" spans="1:260" ht="61" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="32">
+    <row r="10" spans="1:258" ht="72" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="30">
         <v>1</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="16" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="2"/>
@@ -2740,27 +2900,47 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="34"/>
+      <c r="J10" s="63"/>
+      <c r="K10" s="67"/>
+      <c r="L10" s="67"/>
+      <c r="M10" s="67"/>
+      <c r="N10" s="67"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="12"/>
+      <c r="T10" s="12"/>
+      <c r="U10" s="12"/>
+      <c r="V10" s="12"/>
+      <c r="W10" s="12"/>
+      <c r="X10" s="12"/>
+      <c r="Y10" s="12"/>
+      <c r="IQ10" s="13"/>
+      <c r="IR10" s="13"/>
+      <c r="IS10" s="13"/>
+      <c r="IT10" s="13"/>
+      <c r="IU10" s="13"/>
+      <c r="IV10" s="13"/>
+      <c r="IW10" s="13"/>
+      <c r="IX10" s="13"/>
     </row>
-    <row r="11" spans="1:260" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="62" t="s">
+    <row r="11" spans="1:258" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="61" t="s">
+      <c r="B11" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="46"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="47"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="68"/>
+      <c r="L11" s="68"/>
+      <c r="M11" s="68"/>
+      <c r="N11" s="68"/>
       <c r="O11" s="12"/>
       <c r="P11" s="12"/>
       <c r="Q11" s="12"/>
@@ -2772,8 +2952,8 @@
       <c r="W11" s="12"/>
       <c r="X11" s="12"/>
       <c r="Y11" s="12"/>
-      <c r="Z11" s="12"/>
-      <c r="AA11" s="12"/>
+      <c r="Z11" s="13"/>
+      <c r="AA11" s="13"/>
       <c r="AB11" s="13"/>
       <c r="AC11" s="13"/>
       <c r="AD11" s="13"/>
@@ -3005,11 +3185,9 @@
       <c r="IV11" s="13"/>
       <c r="IW11" s="13"/>
       <c r="IX11" s="13"/>
-      <c r="IY11" s="13"/>
-      <c r="IZ11" s="13"/>
     </row>
-    <row r="12" spans="1:260" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="35"/>
+    <row r="12" spans="1:258" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="33"/>
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -3018,43 +3196,83 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
-      <c r="J12" s="36"/>
+      <c r="J12" s="64"/>
+      <c r="K12" s="69"/>
+      <c r="L12" s="69"/>
+      <c r="M12" s="69"/>
+      <c r="N12" s="69"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="12"/>
+      <c r="U12" s="12"/>
+      <c r="V12" s="12"/>
+      <c r="W12" s="12"/>
+      <c r="X12" s="12"/>
+      <c r="Y12" s="12"/>
+      <c r="IQ12" s="13"/>
+      <c r="IR12" s="13"/>
+      <c r="IS12" s="13"/>
+      <c r="IT12" s="13"/>
+      <c r="IU12" s="13"/>
+      <c r="IV12" s="13"/>
+      <c r="IW12" s="13"/>
+      <c r="IX12" s="13"/>
     </row>
-    <row r="13" spans="1:260" ht="46" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32">
+    <row r="13" spans="1:258" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="30">
         <v>1</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="16"/>
+      <c r="C13" s="15"/>
       <c r="D13" s="10"/>
       <c r="E13" s="9"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
-      <c r="J13" s="34"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="67"/>
+      <c r="L13" s="67"/>
+      <c r="M13" s="67"/>
+      <c r="N13" s="67"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="12"/>
+      <c r="U13" s="12"/>
+      <c r="V13" s="12"/>
+      <c r="W13" s="12"/>
+      <c r="X13" s="12"/>
+      <c r="Y13" s="12"/>
+      <c r="IQ13" s="13"/>
+      <c r="IR13" s="13"/>
+      <c r="IS13" s="13"/>
+      <c r="IT13" s="13"/>
+      <c r="IU13" s="13"/>
+      <c r="IV13" s="13"/>
+      <c r="IW13" s="13"/>
+      <c r="IX13" s="13"/>
     </row>
-    <row r="14" spans="1:260" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="62" t="s">
+    <row r="14" spans="1:258" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="61" t="s">
+      <c r="B14" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="46"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="47"/>
-      <c r="J14" s="48"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="53"/>
+      <c r="K14" s="68"/>
+      <c r="L14" s="68"/>
+      <c r="M14" s="68"/>
+      <c r="N14" s="68"/>
       <c r="O14" s="12"/>
       <c r="P14" s="12"/>
       <c r="Q14" s="12"/>
@@ -3066,8 +3284,8 @@
       <c r="W14" s="12"/>
       <c r="X14" s="12"/>
       <c r="Y14" s="12"/>
-      <c r="Z14" s="12"/>
-      <c r="AA14" s="12"/>
+      <c r="Z14" s="13"/>
+      <c r="AA14" s="13"/>
       <c r="AB14" s="13"/>
       <c r="AC14" s="13"/>
       <c r="AD14" s="13"/>
@@ -3299,11 +3517,9 @@
       <c r="IV14" s="13"/>
       <c r="IW14" s="13"/>
       <c r="IX14" s="13"/>
-      <c r="IY14" s="13"/>
-      <c r="IZ14" s="13"/>
     </row>
-    <row r="15" spans="1:260" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="35"/>
+    <row r="15" spans="1:258" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="33"/>
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -3312,13 +3528,33 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
-      <c r="J15" s="36"/>
+      <c r="J15" s="64"/>
+      <c r="K15" s="69"/>
+      <c r="L15" s="69"/>
+      <c r="M15" s="69"/>
+      <c r="N15" s="69"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="12"/>
+      <c r="U15" s="12"/>
+      <c r="V15" s="12"/>
+      <c r="W15" s="12"/>
+      <c r="X15" s="12"/>
+      <c r="Y15" s="12"/>
+      <c r="IQ15" s="13"/>
+      <c r="IR15" s="13"/>
+      <c r="IS15" s="13"/>
+      <c r="IT15" s="13"/>
+      <c r="IU15" s="13"/>
+      <c r="IV15" s="13"/>
+      <c r="IW15" s="13"/>
+      <c r="IX15" s="13"/>
     </row>
-    <row r="16" spans="1:260" ht="46" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="32">
+    <row r="16" spans="1:258" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="30">
         <v>1</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="16" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="2"/>
@@ -3328,27 +3564,47 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-      <c r="J16" s="34"/>
+      <c r="J16" s="63"/>
+      <c r="K16" s="67"/>
+      <c r="L16" s="67"/>
+      <c r="M16" s="67"/>
+      <c r="N16" s="67"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="12"/>
+      <c r="T16" s="12"/>
+      <c r="U16" s="12"/>
+      <c r="V16" s="12"/>
+      <c r="W16" s="12"/>
+      <c r="X16" s="12"/>
+      <c r="Y16" s="12"/>
+      <c r="IQ16" s="13"/>
+      <c r="IR16" s="13"/>
+      <c r="IS16" s="13"/>
+      <c r="IT16" s="13"/>
+      <c r="IU16" s="13"/>
+      <c r="IV16" s="13"/>
+      <c r="IW16" s="13"/>
+      <c r="IX16" s="13"/>
     </row>
-    <row r="17" spans="1:260" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="62" t="s">
+    <row r="17" spans="1:258" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="61" t="s">
+      <c r="B17" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="48"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="53"/>
+      <c r="K17" s="68"/>
+      <c r="L17" s="68"/>
+      <c r="M17" s="68"/>
+      <c r="N17" s="68"/>
       <c r="O17" s="12"/>
       <c r="P17" s="12"/>
       <c r="Q17" s="12"/>
@@ -3360,8 +3616,8 @@
       <c r="W17" s="12"/>
       <c r="X17" s="12"/>
       <c r="Y17" s="12"/>
-      <c r="Z17" s="12"/>
-      <c r="AA17" s="12"/>
+      <c r="Z17" s="13"/>
+      <c r="AA17" s="13"/>
       <c r="AB17" s="13"/>
       <c r="AC17" s="13"/>
       <c r="AD17" s="13"/>
@@ -3593,11 +3849,9 @@
       <c r="IV17" s="13"/>
       <c r="IW17" s="13"/>
       <c r="IX17" s="13"/>
-      <c r="IY17" s="13"/>
-      <c r="IZ17" s="13"/>
     </row>
-    <row r="18" spans="1:260" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="35"/>
+    <row r="18" spans="1:258" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="33"/>
       <c r="B18" s="3" t="s">
         <v>28</v>
       </c>
@@ -3608,26 +3862,50 @@
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
-      <c r="J18" s="31"/>
+      <c r="J18" s="65"/>
+      <c r="K18" s="69"/>
+      <c r="L18" s="69"/>
+      <c r="M18" s="69"/>
+      <c r="N18" s="69"/>
+      <c r="R18" s="12"/>
+      <c r="S18" s="12"/>
+      <c r="T18" s="12"/>
+      <c r="U18" s="12"/>
+      <c r="V18" s="12"/>
+      <c r="W18" s="12"/>
+      <c r="X18" s="12"/>
+      <c r="Y18" s="12"/>
+      <c r="IQ18" s="13"/>
+      <c r="IR18" s="13"/>
+      <c r="IS18" s="13"/>
+      <c r="IT18" s="13"/>
+      <c r="IU18" s="13"/>
+      <c r="IV18" s="13"/>
+      <c r="IW18" s="13"/>
+      <c r="IX18" s="13"/>
     </row>
-    <row r="19" spans="1:260" ht="30" x14ac:dyDescent="0.2">
-      <c r="A19" s="32">
+    <row r="19" spans="1:258" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="30">
         <v>1</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
       <c r="G19" s="14"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="34"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="32"/>
+      <c r="L19" s="32"/>
+      <c r="M19" s="32"/>
+      <c r="N19" s="32"/>
     </row>
-    <row r="20" spans="1:260" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="35"/>
+    <row r="20" spans="1:258" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="33"/>
       <c r="B20" s="3" t="s">
         <v>30</v>
       </c>
@@ -3638,28 +3916,36 @@
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
-      <c r="J20" s="36"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="34"/>
+      <c r="M20" s="34"/>
+      <c r="N20" s="34"/>
     </row>
-    <row r="21" spans="1:260" x14ac:dyDescent="0.2">
-      <c r="A21" s="37">
+    <row r="21" spans="1:258" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="35">
         <v>2</v>
       </c>
-      <c r="B21" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
+      <c r="B21" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
       <c r="H21" s="14"/>
       <c r="I21" s="2"/>
-      <c r="J21" s="34"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="32"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="32"/>
+      <c r="N21" s="32"/>
     </row>
-    <row r="22" spans="1:260" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="35"/>
+    <row r="22" spans="1:258" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="33"/>
       <c r="B22" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
@@ -3668,28 +3954,36 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
-      <c r="J22" s="36"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="70"/>
+      <c r="L22" s="70"/>
+      <c r="M22" s="70"/>
+      <c r="N22" s="70"/>
     </row>
-    <row r="23" spans="1:260" x14ac:dyDescent="0.2">
-      <c r="A23" s="37">
+    <row r="23" spans="1:258" x14ac:dyDescent="0.25">
+      <c r="A23" s="35">
         <v>3</v>
       </c>
-      <c r="B23" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
+      <c r="B23" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="15"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
       <c r="I23" s="14"/>
-      <c r="J23" s="38"/>
+      <c r="J23" s="73"/>
+      <c r="K23" s="56"/>
+      <c r="L23" s="56"/>
+      <c r="M23" s="56"/>
+      <c r="N23" s="56"/>
     </row>
-    <row r="24" spans="1:260" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="35"/>
+    <row r="24" spans="1:258" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="33"/>
       <c r="B24" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -3698,56 +3992,64 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
-      <c r="J24" s="36"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="66"/>
+      <c r="L24" s="66"/>
+      <c r="M24" s="66"/>
+      <c r="N24" s="66"/>
     </row>
-    <row r="25" spans="1:260" ht="31" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="32">
+    <row r="25" spans="1:258" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="30">
         <v>4</v>
       </c>
-      <c r="B25" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="39"/>
+      <c r="B25" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="15"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="74"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="56"/>
+      <c r="M25" s="56"/>
+      <c r="N25" s="56"/>
     </row>
-    <row r="26" spans="1:260" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="62" t="s">
+    <row r="26" spans="1:258" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="61" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" s="46"/>
-      <c r="D26" s="47"/>
-      <c r="E26" s="47"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="47"/>
-      <c r="I26" s="47"/>
-      <c r="J26" s="48"/>
-      <c r="K26" s="12"/>
-      <c r="L26" s="12"/>
-      <c r="M26" s="12"/>
-      <c r="N26" s="12"/>
+      <c r="B26" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="52"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="53"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="54"/>
+      <c r="K26" s="71"/>
+      <c r="L26" s="72"/>
+      <c r="M26" s="72"/>
+      <c r="N26" s="72"/>
       <c r="O26" s="12"/>
       <c r="P26" s="12"/>
       <c r="Q26" s="12"/>
-      <c r="R26" s="12"/>
-      <c r="S26" s="12"/>
-      <c r="T26" s="12"/>
-      <c r="U26" s="12"/>
-      <c r="V26" s="12"/>
-      <c r="W26" s="12"/>
-      <c r="X26" s="12"/>
-      <c r="Y26" s="12"/>
-      <c r="Z26" s="12"/>
-      <c r="AA26" s="12"/>
+      <c r="R26" s="13"/>
+      <c r="S26" s="13"/>
+      <c r="T26" s="13"/>
+      <c r="U26" s="13"/>
+      <c r="V26" s="13"/>
+      <c r="W26" s="13"/>
+      <c r="X26" s="13"/>
+      <c r="Y26" s="13"/>
+      <c r="Z26" s="13"/>
+      <c r="AA26" s="13"/>
       <c r="AB26" s="13"/>
       <c r="AC26" s="13"/>
       <c r="AD26" s="13"/>
@@ -3971,20 +4273,10 @@
       <c r="IN26" s="13"/>
       <c r="IO26" s="13"/>
       <c r="IP26" s="13"/>
-      <c r="IQ26" s="13"/>
-      <c r="IR26" s="13"/>
-      <c r="IS26" s="13"/>
-      <c r="IT26" s="13"/>
-      <c r="IU26" s="13"/>
-      <c r="IV26" s="13"/>
-      <c r="IW26" s="13"/>
-      <c r="IX26" s="13"/>
-      <c r="IY26" s="13"/>
-      <c r="IZ26" s="13"/>
     </row>
-    <row r="27" spans="1:260" x14ac:dyDescent="0.2">
-      <c r="A27" s="35"/>
-      <c r="B27" s="19"/>
+    <row r="27" spans="1:258" x14ac:dyDescent="0.25">
+      <c r="A27" s="33"/>
+      <c r="B27" s="18"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
@@ -3992,35 +4284,103 @@
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
-      <c r="J27" s="31"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="66"/>
+      <c r="L27" s="66"/>
+      <c r="M27" s="66"/>
+      <c r="N27" s="66"/>
     </row>
-    <row r="28" spans="1:260" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="40">
+    <row r="28" spans="1:258" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="75">
         <v>1</v>
       </c>
-      <c r="B28" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" s="41"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="41"/>
-      <c r="I28" s="42"/>
-      <c r="J28" s="43"/>
+      <c r="B28" s="76" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="77"/>
+      <c r="J28" s="78"/>
+      <c r="K28" s="79"/>
+      <c r="L28" s="79"/>
+      <c r="M28" s="80"/>
+      <c r="N28" s="80"/>
+    </row>
+    <row r="29" spans="1:258" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="75">
+        <v>2</v>
+      </c>
+      <c r="B29" s="76" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="81"/>
+      <c r="D29" s="81"/>
+      <c r="E29" s="81"/>
+      <c r="F29" s="81"/>
+      <c r="G29" s="81"/>
+      <c r="H29" s="81"/>
+      <c r="I29" s="81"/>
+      <c r="J29" s="81"/>
+      <c r="K29" s="56"/>
+      <c r="L29" s="56"/>
+      <c r="M29" s="79"/>
+      <c r="N29" s="56"/>
+    </row>
+    <row r="30" spans="1:258" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="75">
+        <v>3</v>
+      </c>
+      <c r="B30" s="76" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="81"/>
+      <c r="D30" s="81"/>
+      <c r="E30" s="81"/>
+      <c r="F30" s="81"/>
+      <c r="G30" s="81"/>
+      <c r="H30" s="81"/>
+      <c r="I30" s="81"/>
+      <c r="J30" s="81"/>
+      <c r="K30" s="56"/>
+      <c r="L30" s="56"/>
+      <c r="M30" s="56"/>
+      <c r="N30" s="79"/>
+    </row>
+    <row r="31" spans="1:258" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="81"/>
+      <c r="B31" s="81"/>
+      <c r="C31" s="81"/>
+      <c r="D31" s="81"/>
+      <c r="E31" s="81"/>
+      <c r="F31" s="81"/>
+      <c r="G31" s="81"/>
+      <c r="H31" s="81"/>
+      <c r="I31" s="81"/>
+      <c r="J31" s="81"/>
+      <c r="K31" s="56"/>
+      <c r="L31" s="56"/>
+      <c r="M31" s="56"/>
+      <c r="N31" s="56"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="13">
+    <mergeCell ref="C17:J17"/>
+    <mergeCell ref="C26:J26"/>
+    <mergeCell ref="C11:J11"/>
+    <mergeCell ref="C14:J14"/>
+    <mergeCell ref="K1:N2"/>
+    <mergeCell ref="K8:N8"/>
+    <mergeCell ref="K26:N26"/>
+    <mergeCell ref="K5:N5"/>
     <mergeCell ref="A1:B3"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="C1:G2"/>
     <mergeCell ref="C5:J5"/>
     <mergeCell ref="C8:J8"/>
-    <mergeCell ref="C17:J17"/>
-    <mergeCell ref="C26:J26"/>
-    <mergeCell ref="C11:J11"/>
-    <mergeCell ref="C14:J14"/>
   </mergeCells>
   <pageMargins left="0.21" right="0.28000000000000003" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="50" orientation="landscape" r:id="rId1"/>

</xml_diff>